<commit_message>
Added new thesis project to repro
</commit_message>
<xml_diff>
--- a/TheTrial/Docs/ProgressTracking.xlsx
+++ b/TheTrial/Docs/ProgressTracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Guildhall\TheTrial\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF273F5-3242-4E79-9338-A5F566562CA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81D1506-BD4E-4830-9439-9E9E7477FC7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{603EAEDC-D363-457D-B800-748B64D3B649}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{603EAEDC-D363-457D-B800-748B64D3B649}"/>
   </bookViews>
   <sheets>
     <sheet name="Milestones" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="184">
   <si>
     <t>Task ID</t>
   </si>
@@ -582,6 +582,12 @@
   </si>
   <si>
     <t>Write save state to XML</t>
+  </si>
+  <si>
+    <t>Update Ability Select Menu to be navigable with mouse</t>
+  </si>
+  <si>
+    <t>Display item stats when hovered</t>
   </si>
 </sst>
 </file>
@@ -1022,7 +1028,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="75">
+  <dxfs count="78">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2396,11 +2432,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D356B3F-B2FC-4492-B6C6-3B09C1815C2E}">
-  <dimension ref="A1:I103"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F98" sqref="F96:F98"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A103" activeCellId="4" sqref="A95:A96 A99:A100 A104:A105 A102 A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -3760,7 +3796,7 @@
       </c>
       <c r="F57" s="59" t="str">
         <f>"Total Hours Completed: " &amp; SUM(D59:D89)</f>
-        <v>Total Hours Completed: 22</v>
+        <v>Total Hours Completed: 25.5</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="40" customFormat="1" ht="90" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4281,7 +4317,7 @@
       </c>
       <c r="B79" s="28" t="str">
         <f>IF( ISBLANK($A79), "", VLOOKUP($A79,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v>Not Started</v>
+        <v>Completed</v>
       </c>
       <c r="C79" s="28">
         <f>IF( ISBLANK($A79), "", VLOOKUP($A79,Backlog!$A$2:$F$207, COLUMN()))</f>
@@ -4289,7 +4325,7 @@
       </c>
       <c r="D79" s="28">
         <f>IF( ISBLANK($A79), "", VLOOKUP($A79,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E79" s="28" t="str">
         <f>IF( ISBLANK($A79), "", VLOOKUP($A79,Backlog!$A$2:$F$207, COLUMN()))</f>
@@ -4306,7 +4342,7 @@
       </c>
       <c r="B80" s="28" t="str">
         <f>IF( ISBLANK($A80), "", VLOOKUP($A80,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v>Not Started</v>
+        <v>Completed</v>
       </c>
       <c r="C80" s="28">
         <f>IF( ISBLANK($A80), "", VLOOKUP($A80,Backlog!$A$2:$F$207, COLUMN()))</f>
@@ -4314,7 +4350,7 @@
       </c>
       <c r="D80" s="28">
         <f>IF( ISBLANK($A80), "", VLOOKUP($A80,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E80" s="28" t="str">
         <f>IF( ISBLANK($A80), "", VLOOKUP($A80,Backlog!$A$2:$F$207, COLUMN()))</f>
@@ -4558,8 +4594,8 @@
         <v>44032</v>
       </c>
       <c r="F91" s="79" t="str">
-        <f>"Total Hours Completed: " &amp; SUM(D93:D123)</f>
-        <v>Total Hours Completed: 0</v>
+        <f>"Total Hours Completed: " &amp; SUM(D93:D105)</f>
+        <v>Total Hours Completed: 12</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -4643,7 +4679,7 @@
       </c>
       <c r="B95" s="39" t="str">
         <f>IF( ISBLANK($A95), "", VLOOKUP($A95,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v>Not Started</v>
+        <v>Completed</v>
       </c>
       <c r="C95" s="39">
         <f>IF( ISBLANK($A95), "", VLOOKUP($A95,Backlog!$A$2:$F$207, COLUMN()))</f>
@@ -4651,7 +4687,7 @@
       </c>
       <c r="D95" s="39">
         <f>IF( ISBLANK($A95), "", VLOOKUP($A95,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E95" s="39" t="str">
         <f>IF( ISBLANK($A95), "", VLOOKUP($A95,Backlog!$A$2:$F$207, COLUMN()))</f>
@@ -4668,7 +4704,7 @@
       </c>
       <c r="B96" s="39" t="str">
         <f>IF( ISBLANK($A96), "", VLOOKUP($A96,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v>Not Started</v>
+        <v>Completed</v>
       </c>
       <c r="C96" s="39">
         <f>IF( ISBLANK($A96), "", VLOOKUP($A96,Backlog!$A$2:$F$207, COLUMN()))</f>
@@ -4676,7 +4712,7 @@
       </c>
       <c r="D96" s="39">
         <f>IF( ISBLANK($A96), "", VLOOKUP($A96,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E96" s="39" t="str">
         <f>IF( ISBLANK($A96), "", VLOOKUP($A96,Backlog!$A$2:$F$207, COLUMN()))</f>
@@ -4743,7 +4779,7 @@
       </c>
       <c r="B99" s="39" t="str">
         <f>IF( ISBLANK($A99), "", VLOOKUP($A99,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v>Not Started</v>
+        <v>Completed</v>
       </c>
       <c r="C99" s="39">
         <f>IF( ISBLANK($A99), "", VLOOKUP($A99,Backlog!$A$2:$F$207, COLUMN()))</f>
@@ -4751,7 +4787,7 @@
       </c>
       <c r="D99" s="39">
         <f>IF( ISBLANK($A99), "", VLOOKUP($A99,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E99" s="39" t="str">
         <f>IF( ISBLANK($A99), "", VLOOKUP($A99,Backlog!$A$2:$F$207, COLUMN()))</f>
@@ -4768,7 +4804,7 @@
       </c>
       <c r="B100" s="39" t="str">
         <f>IF( ISBLANK($A100), "", VLOOKUP($A100,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v>Not Started</v>
+        <v>Completed</v>
       </c>
       <c r="C100" s="39">
         <f>IF( ISBLANK($A100), "", VLOOKUP($A100,Backlog!$A$2:$F$207, COLUMN()))</f>
@@ -4776,7 +4812,7 @@
       </c>
       <c r="D100" s="39">
         <f>IF( ISBLANK($A100), "", VLOOKUP($A100,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E100" s="39" t="str">
         <f>IF( ISBLANK($A100), "", VLOOKUP($A100,Backlog!$A$2:$F$207, COLUMN()))</f>
@@ -4818,7 +4854,7 @@
       </c>
       <c r="B102" s="39" t="str">
         <f>IF( ISBLANK($A102), "", VLOOKUP($A102,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v>Not Started</v>
+        <v>Completed</v>
       </c>
       <c r="C102" s="39">
         <f>IF( ISBLANK($A102), "", VLOOKUP($A102,Backlog!$A$2:$F$207, COLUMN()))</f>
@@ -4826,7 +4862,7 @@
       </c>
       <c r="D102" s="39">
         <f>IF( ISBLANK($A102), "", VLOOKUP($A102,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E102" s="39" t="str">
         <f>IF( ISBLANK($A102), "", VLOOKUP($A102,Backlog!$A$2:$F$207, COLUMN()))</f>
@@ -4843,7 +4879,7 @@
       </c>
       <c r="B103" s="39" t="str">
         <f>IF( ISBLANK($A103), "", VLOOKUP($A103,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v>Not Started</v>
+        <v>Completed</v>
       </c>
       <c r="C103" s="39">
         <f>IF( ISBLANK($A103), "", VLOOKUP($A103,Backlog!$A$2:$F$207, COLUMN()))</f>
@@ -4851,7 +4887,7 @@
       </c>
       <c r="D103" s="39">
         <f>IF( ISBLANK($A103), "", VLOOKUP($A103,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103" s="39" t="str">
         <f>IF( ISBLANK($A103), "", VLOOKUP($A103,Backlog!$A$2:$F$207, COLUMN()))</f>
@@ -4862,112 +4898,162 @@
         <v>Bug Fixing</v>
       </c>
     </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
+        <v>102</v>
+      </c>
+      <c r="B104" s="39" t="str">
+        <f>IF( ISBLANK($A104), "", VLOOKUP($A104,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>Completed</v>
+      </c>
+      <c r="C104" s="39">
+        <f>IF( ISBLANK($A104), "", VLOOKUP($A104,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>2</v>
+      </c>
+      <c r="D104" s="39">
+        <f>IF( ISBLANK($A104), "", VLOOKUP($A104,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>2</v>
+      </c>
+      <c r="E104" s="39" t="str">
+        <f>IF( ISBLANK($A104), "", VLOOKUP($A104,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>-</v>
+      </c>
+      <c r="F104" s="30" t="str">
+        <f>IF( ISBLANK($A104), "", VLOOKUP($A104,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>Update Ability Select Menu to be navigable with mouse</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
+        <v>103</v>
+      </c>
+      <c r="B105" s="39" t="str">
+        <f>IF( ISBLANK($A105), "", VLOOKUP($A105,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>Completed</v>
+      </c>
+      <c r="C105" s="39">
+        <f>IF( ISBLANK($A105), "", VLOOKUP($A105,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>1</v>
+      </c>
+      <c r="D105" s="39">
+        <f>IF( ISBLANK($A105), "", VLOOKUP($A105,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>1.5</v>
+      </c>
+      <c r="E105" s="39" t="str">
+        <f>IF( ISBLANK($A105), "", VLOOKUP($A105,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>-</v>
+      </c>
+      <c r="F105" s="30" t="str">
+        <f>IF( ISBLANK($A105), "", VLOOKUP($A105,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>Display item stats when hovered</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B3 B29:B30">
-    <cfRule type="cellIs" dxfId="74" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="29" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="30" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="31" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:F4 B4:B28">
-    <cfRule type="cellIs" dxfId="71" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="26" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="27" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="28" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:B55">
-    <cfRule type="cellIs" dxfId="68" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="20" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="21" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="22" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F87 A89">
-    <cfRule type="expression" dxfId="65" priority="19">
+    <cfRule type="expression" dxfId="68" priority="19">
       <formula>$B1="Deleted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57:B58">
-    <cfRule type="cellIs" dxfId="64" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="16" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="17" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="18" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59:B87">
-    <cfRule type="cellIs" dxfId="61" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="13" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="14" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="15" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88:F89">
-    <cfRule type="expression" dxfId="58" priority="12">
+    <cfRule type="expression" dxfId="61" priority="12">
       <formula>$B88="Deleted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88:B89">
-    <cfRule type="cellIs" dxfId="57" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="9" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="10" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="11" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91:F91">
-    <cfRule type="expression" dxfId="54" priority="8">
+    <cfRule type="expression" dxfId="57" priority="8">
       <formula>$B91="Deleted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="cellIs" dxfId="53" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="5" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="6" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="7" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B92:F103">
-    <cfRule type="expression" dxfId="50" priority="4">
+  <conditionalFormatting sqref="B92:F105">
+    <cfRule type="expression" dxfId="53" priority="4">
       <formula>$B92="Deleted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B92:B103">
-    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
+  <conditionalFormatting sqref="B92:B105">
+    <cfRule type="cellIs" dxfId="52" priority="1" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="2" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="3" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4978,10 +5064,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B1D0D5-8BE9-4C2F-A748-65963B5C1812}">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6827,106 +6913,266 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B79" s="28" t="str">
-        <f>IF( ISBLANK($A79), "", VLOOKUP($A79,Backlog!$A$2:$F$203, COLUMN()))</f>
-        <v/>
-      </c>
-      <c r="C79" s="28" t="str">
-        <f>IF( ISBLANK($A79), "", VLOOKUP($A79,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v/>
-      </c>
-      <c r="D79" s="28" t="str">
-        <f>IF( ISBLANK($A79), "", VLOOKUP($A79,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v/>
-      </c>
-      <c r="E79" s="28" t="str">
-        <f>IF( ISBLANK($A79), "", VLOOKUP($A79,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v/>
-      </c>
-      <c r="F79" s="31" t="str">
-        <f>IF( ISBLANK($A79), "", VLOOKUP($A79,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v/>
+      <c r="A79" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B79" s="42">
+        <v>44032</v>
+      </c>
+      <c r="C79" s="43"/>
+      <c r="D79" s="41"/>
+      <c r="E79" s="43"/>
+      <c r="F79" s="44" t="str">
+        <f>"Hours Worked: " &amp; SUM(D80:D88)</f>
+        <v>Hours Worked: 12</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>90</v>
+      </c>
       <c r="B80" s="28" t="str">
         <f>IF( ISBLANK($A80), "", VLOOKUP($A80,Backlog!$A$2:$F$203, COLUMN()))</f>
-        <v/>
-      </c>
-      <c r="C80" s="28" t="str">
+        <v>Completed</v>
+      </c>
+      <c r="C80" s="28">
         <f>IF( ISBLANK($A80), "", VLOOKUP($A80,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v/>
-      </c>
-      <c r="D80" s="28" t="str">
+        <v>2</v>
+      </c>
+      <c r="D80" s="28">
         <f>IF( ISBLANK($A80), "", VLOOKUP($A80,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="E80" s="28" t="str">
         <f>IF( ISBLANK($A80), "", VLOOKUP($A80,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F80" s="31" t="str">
         <f>IF( ISBLANK($A80), "", VLOOKUP($A80,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+        <v>Get Audio assets for: BGM, PlayerAttack, EnemyAttack, pick up Item</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>91</v>
+      </c>
       <c r="B81" s="28" t="str">
         <f>IF( ISBLANK($A81), "", VLOOKUP($A81,Backlog!$A$2:$F$203, COLUMN()))</f>
-        <v/>
-      </c>
-      <c r="C81" s="28" t="str">
+        <v>Completed</v>
+      </c>
+      <c r="C81" s="28">
         <f>IF( ISBLANK($A81), "", VLOOKUP($A81,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v/>
-      </c>
-      <c r="D81" s="28" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="D81" s="28">
         <f>IF( ISBLANK($A81), "", VLOOKUP($A81,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v/>
+        <v>1.5</v>
       </c>
       <c r="E81" s="28" t="str">
         <f>IF( ISBLANK($A81), "", VLOOKUP($A81,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F81" s="31" t="str">
         <f>IF( ISBLANK($A81), "", VLOOKUP($A81,Backlog!$A$2:$F$207, COLUMN()))</f>
-        <v/>
+        <v>Implement playing audio on actions</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>99</v>
+      </c>
+      <c r="B82" s="28" t="str">
+        <f>IF( ISBLANK($A82), "", VLOOKUP($A82,Backlog!$A$2:$F$203, COLUMN()))</f>
+        <v>Completed</v>
+      </c>
+      <c r="C82" s="28">
+        <f>IF( ISBLANK($A82), "", VLOOKUP($A82,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>2</v>
+      </c>
+      <c r="D82" s="28">
+        <f>IF( ISBLANK($A82), "", VLOOKUP($A82,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>2</v>
+      </c>
+      <c r="E82" s="28" t="str">
+        <f>IF( ISBLANK($A82), "", VLOOKUP($A82,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>-</v>
+      </c>
+      <c r="F82" s="31" t="str">
+        <f>IF( ISBLANK($A82), "", VLOOKUP($A82,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>Create 2 Additional Maps</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>100</v>
+      </c>
+      <c r="B83" s="28" t="str">
+        <f>IF( ISBLANK($A83), "", VLOOKUP($A83,Backlog!$A$2:$F$203, COLUMN()))</f>
+        <v>Completed</v>
+      </c>
+      <c r="C83" s="28">
+        <f>IF( ISBLANK($A83), "", VLOOKUP($A83,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>2</v>
+      </c>
+      <c r="D83" s="28">
+        <f>IF( ISBLANK($A83), "", VLOOKUP($A83,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>0.5</v>
+      </c>
+      <c r="E83" s="28" t="str">
+        <f>IF( ISBLANK($A83), "", VLOOKUP($A83,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>-</v>
+      </c>
+      <c r="F83" s="31" t="str">
+        <f>IF( ISBLANK($A83), "", VLOOKUP($A83,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>Create Additional Items</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>54</v>
+      </c>
+      <c r="B84" s="28" t="str">
+        <f>IF( ISBLANK($A84), "", VLOOKUP($A84,Backlog!$A$2:$F$203, COLUMN()))</f>
+        <v>Completed</v>
+      </c>
+      <c r="C84" s="28">
+        <f>IF( ISBLANK($A84), "", VLOOKUP($A84,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>10</v>
+      </c>
+      <c r="D84" s="28">
+        <f>IF( ISBLANK($A84), "", VLOOKUP($A84,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>1.5</v>
+      </c>
+      <c r="E84" s="28" t="str">
+        <f>IF( ISBLANK($A84), "", VLOOKUP($A84,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>-</v>
+      </c>
+      <c r="F84" s="31" t="str">
+        <f>IF( ISBLANK($A84), "", VLOOKUP($A84,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>Polish</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>55</v>
+      </c>
+      <c r="B85" s="28" t="str">
+        <f>IF( ISBLANK($A85), "", VLOOKUP($A85,Backlog!$A$2:$F$203, COLUMN()))</f>
+        <v>Completed</v>
+      </c>
+      <c r="C85" s="28">
+        <f>IF( ISBLANK($A85), "", VLOOKUP($A85,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>10</v>
+      </c>
+      <c r="D85" s="28">
+        <f>IF( ISBLANK($A85), "", VLOOKUP($A85,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>1</v>
+      </c>
+      <c r="E85" s="28" t="str">
+        <f>IF( ISBLANK($A85), "", VLOOKUP($A85,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>-</v>
+      </c>
+      <c r="F85" s="31" t="str">
+        <f>IF( ISBLANK($A85), "", VLOOKUP($A85,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>Bug Fixing</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>102</v>
+      </c>
+      <c r="B86" s="28" t="str">
+        <f>IF( ISBLANK($A86), "", VLOOKUP($A86,Backlog!$A$2:$F$203, COLUMN()))</f>
+        <v>Completed</v>
+      </c>
+      <c r="C86" s="28">
+        <f>IF( ISBLANK($A86), "", VLOOKUP($A86,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>2</v>
+      </c>
+      <c r="D86" s="28">
+        <f>IF( ISBLANK($A86), "", VLOOKUP($A86,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>2</v>
+      </c>
+      <c r="E86" s="28" t="str">
+        <f>IF( ISBLANK($A86), "", VLOOKUP($A86,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>-</v>
+      </c>
+      <c r="F86" s="31" t="str">
+        <f>IF( ISBLANK($A86), "", VLOOKUP($A86,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>Update Ability Select Menu to be navigable with mouse</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>103</v>
+      </c>
+      <c r="B87" s="28" t="str">
+        <f>IF( ISBLANK($A87), "", VLOOKUP($A87,Backlog!$A$2:$F$203, COLUMN()))</f>
+        <v>Completed</v>
+      </c>
+      <c r="C87" s="28">
+        <f>IF( ISBLANK($A87), "", VLOOKUP($A87,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>1</v>
+      </c>
+      <c r="D87" s="28">
+        <f>IF( ISBLANK($A87), "", VLOOKUP($A87,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>1.5</v>
+      </c>
+      <c r="E87" s="28" t="str">
+        <f>IF( ISBLANK($A87), "", VLOOKUP($A87,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>-</v>
+      </c>
+      <c r="F87" s="31" t="str">
+        <f>IF( ISBLANK($A87), "", VLOOKUP($A87,Backlog!$A$2:$F$207, COLUMN()))</f>
+        <v>Display item stats when hovered</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="cellIs" dxfId="46" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="46" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="47" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="48" operator="equal">
+      <formula>"Not Started"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B10 B22:B35 B62:B66 B68 B70:B78 B80:B87">
+    <cfRule type="cellIs" dxfId="46" priority="43" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="45" priority="44" operator="equal">
-      <formula>"In Progress"</formula>
+      <formula>"Completed"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="44" priority="45" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B10 B22:B35 B62:B66 B68 B70:B81">
+  <conditionalFormatting sqref="B11">
     <cfRule type="cellIs" dxfId="43" priority="40" operator="equal">
-      <formula>"In Progress"</formula>
+      <formula>"Completed"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="42" priority="41" operator="equal">
-      <formula>"Completed"</formula>
+      <formula>"In Progress"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="41" priority="42" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11">
+  <conditionalFormatting sqref="B13:B20">
     <cfRule type="cellIs" dxfId="40" priority="37" operator="equal">
-      <formula>"Completed"</formula>
+      <formula>"In Progress"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
-      <formula>"In Progress"</formula>
+      <formula>"Completed"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:B20">
+  <conditionalFormatting sqref="B12">
     <cfRule type="cellIs" dxfId="37" priority="34" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
@@ -6937,18 +7183,18 @@
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12">
+  <conditionalFormatting sqref="B21">
     <cfRule type="cellIs" dxfId="34" priority="31" operator="equal">
-      <formula>"In Progress"</formula>
+      <formula>"Completed"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="33" priority="32" operator="equal">
-      <formula>"Completed"</formula>
+      <formula>"In Progress"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="32" priority="33" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21">
+  <conditionalFormatting sqref="B36">
     <cfRule type="cellIs" dxfId="31" priority="28" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
@@ -6959,62 +7205,62 @@
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B36">
-    <cfRule type="cellIs" dxfId="28" priority="25" operator="equal">
+  <conditionalFormatting sqref="B37:B50">
+    <cfRule type="cellIs" dxfId="28" priority="22" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="24" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B37:B50">
+  <conditionalFormatting sqref="B51">
     <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
-      <formula>"In Progress"</formula>
+      <formula>"Completed"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
-      <formula>"Completed"</formula>
+      <formula>"In Progress"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B51">
+  <conditionalFormatting sqref="B52:B60">
     <cfRule type="cellIs" dxfId="22" priority="16" operator="equal">
-      <formula>"Completed"</formula>
+      <formula>"In Progress"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="21" priority="17" operator="equal">
-      <formula>"In Progress"</formula>
+      <formula>"Completed"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B52:B60">
+  <conditionalFormatting sqref="B61">
     <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
-      <formula>"In Progress"</formula>
+      <formula>"Completed"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
-      <formula>"Completed"</formula>
+      <formula>"In Progress"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B61">
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+  <conditionalFormatting sqref="B67">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B67">
+  <conditionalFormatting sqref="B69">
     <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
@@ -7025,14 +7271,14 @@
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B69">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+  <conditionalFormatting sqref="B79">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7045,8 +7291,8 @@
   <dimension ref="A1:F113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8140,12 +8386,14 @@
         <v>54</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="C55" s="20">
         <v>10</v>
       </c>
-      <c r="D55" s="16"/>
+      <c r="D55" s="16">
+        <v>1.5</v>
+      </c>
       <c r="E55" s="13" t="s">
         <v>56</v>
       </c>
@@ -8159,12 +8407,14 @@
         <v>55</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="C56" s="20">
         <v>10</v>
       </c>
-      <c r="D56" s="16"/>
+      <c r="D56" s="16">
+        <v>1</v>
+      </c>
       <c r="E56" s="13" t="s">
         <v>56</v>
       </c>
@@ -8906,9 +9156,12 @@
         <v>90</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="C93" s="13">
+        <v>2</v>
+      </c>
+      <c r="D93" s="8">
         <v>2</v>
       </c>
       <c r="E93" s="13" t="s">
@@ -8924,9 +9177,12 @@
         <v>91</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="C94" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="D94" s="8">
         <v>1.5</v>
       </c>
       <c r="E94" s="13" t="s">
@@ -9093,12 +9349,14 @@
         <v>99</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="C103" s="13">
         <v>2</v>
       </c>
-      <c r="D103" s="8"/>
+      <c r="D103" s="8">
+        <v>2</v>
+      </c>
       <c r="E103" s="13" t="s">
         <v>56</v>
       </c>
@@ -9112,12 +9370,14 @@
         <v>100</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="C104" s="13">
         <v>2</v>
       </c>
-      <c r="D104" s="8"/>
+      <c r="D104" s="8">
+        <v>0.5</v>
+      </c>
       <c r="E104" s="13" t="s">
         <v>56</v>
       </c>
@@ -9145,20 +9405,44 @@
       </c>
     </row>
     <row r="106" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="7"/>
-      <c r="B106" s="13"/>
-      <c r="C106" s="13"/>
-      <c r="D106" s="8"/>
-      <c r="E106" s="13"/>
-      <c r="F106" s="10"/>
+      <c r="A106" s="7">
+        <v>102</v>
+      </c>
+      <c r="B106" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C106" s="13">
+        <v>2</v>
+      </c>
+      <c r="D106" s="8">
+        <v>2</v>
+      </c>
+      <c r="E106" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F106" s="10" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="107" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="7"/>
-      <c r="B107" s="13"/>
-      <c r="C107" s="13"/>
-      <c r="D107" s="8"/>
-      <c r="E107" s="13"/>
-      <c r="F107" s="10"/>
+      <c r="A107" s="7">
+        <v>103</v>
+      </c>
+      <c r="B107" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C107" s="13">
+        <v>1</v>
+      </c>
+      <c r="D107" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="E107" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F107" s="10" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="108" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="7"/>
@@ -9187,7 +9471,7 @@
       </c>
       <c r="D112" s="16">
         <f>SUMIF(B2:B110, "&lt;&gt;Deleted",C2:C110)</f>
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="113" spans="3:4" x14ac:dyDescent="0.25">
@@ -9196,39 +9480,39 @@
       </c>
       <c r="D113" s="16">
         <f>SUM(D2:D110)</f>
-        <v>57.25</v>
+        <v>69.25</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B100 B110:B1048576">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F100">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>$B2="Deleted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101:B109">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A101:F109">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$B101="Deleted"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>